<commit_message>
color coding conv sheet
</commit_message>
<xml_diff>
--- a/Convolution step.xlsx
+++ b/Convolution step.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97e4a261c9dcd839/Dokumente/UniOsnabrueck/Studium/3_Semester/Implementing ANNs with TensorFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{907302FF-8E03-43AD-8F22-E1F4229196F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97BAE4A6-9D87-4F8D-AD1B-29CFCC78D77F}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{907302FF-8E03-43AD-8F22-E1F4229196F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{58B60691-2347-4261-B0B3-93ABEF9ADD88}"/>
   <bookViews>
-    <workbookView xWindow="-21795" yWindow="840" windowWidth="41355" windowHeight="10560" xr2:uid="{58FE3649-9506-4D9D-A2A4-D1252A2EFCF9}"/>
+    <workbookView xWindow="1740" yWindow="-120" windowWidth="49980" windowHeight="21840" xr2:uid="{58FE3649-9506-4D9D-A2A4-D1252A2EFCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Conv2D</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>(kernel_height * kernel_width * number of filters in the previous layer + 1) * number of filters</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Solutions</t>
   </si>
 </sst>
 </file>
@@ -144,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +184,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF159B52"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,15 +227,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,6 +247,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF159B52"/>
       <color rgb="FF6D4789"/>
     </mruColors>
   </colors>
@@ -530,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DCC6FC-142D-4D87-B200-9B80AE162E67}">
   <dimension ref="A2:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,8 +570,8 @@
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -685,43 +716,53 @@
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>20</v>
       </c>
-      <c r="D18">
-        <v>3</v>
+      <c r="D18" s="4">
+        <v>60</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -729,7 +770,7 @@
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>1</v>
       </c>
     </row>
@@ -737,7 +778,7 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" t="b">
+      <c r="B23" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -745,15 +786,15 @@
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="9">
         <f>IF(OR(padding2="zero",padding2="yes"), ROUNDDOWN((x+kernel_x-1-kernel_x)/strides_x +1,0), ROUNDDOWN((x-kernel_x)/strides_x +1,0))</f>
-        <v>7</v>
-      </c>
-      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="9">
         <f>IF(OR(padding2="zero",padding2="yes"), ROUNDDOWN((y+kernel_y-1-kernel_y)/strides_y +1,0), ROUNDDOWN((y-kernel_y)/strides_y +1,0))</f>
-        <v>7</v>
-      </c>
-      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="D25" s="9">
         <f>filters</f>
         <v>1</v>
       </c>
@@ -762,45 +803,54 @@
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="9">
         <f>IF(use_bias, (kernel_x*kernel_y*depth+1)*filters, (kernel_x*kernel_y*depth)*filters)</f>
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>20</v>
       </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C27">
+      <c r="C27" s="9">
         <f>kernel_x</f>
-        <v>3</v>
-      </c>
-      <c r="D27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="10">
         <f>kernel_y</f>
-        <v>3</v>
-      </c>
-      <c r="F27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="10">
         <f>depth</f>
-        <v>3</v>
-      </c>
-      <c r="H27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="9">
         <f>IF(use_bias,1,0)</f>
         <v>1</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="9">
         <f>filters</f>
         <v>1</v>
       </c>

</xml_diff>